<commit_message>
Azuritao listu taskova, sitne izmene u sttyle.css i login.html
</commit_message>
<xml_diff>
--- a/docs/BIM_PROJEKAT_TASK_LIST.xlsx
+++ b/docs/BIM_PROJEKAT_TASK_LIST.xlsx
@@ -19,8 +19,31 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="J23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">uradjeno</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t xml:space="preserve">Petar</t>
   </si>
@@ -46,15 +69,15 @@
     <t xml:space="preserve">Ognjen</t>
   </si>
   <si>
+    <t xml:space="preserve">Luka</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jova</t>
   </si>
   <si>
     <t xml:space="preserve">Nemanja</t>
   </si>
   <si>
-    <t xml:space="preserve">Luka</t>
-  </si>
-  <si>
     <t xml:space="preserve">HTML na web stranici / UI:</t>
   </si>
   <si>
@@ -64,6 +87,9 @@
     <t xml:space="preserve">templates/index.html</t>
   </si>
   <si>
+    <t xml:space="preserve">pomoc Petru</t>
+  </si>
+  <si>
     <t xml:space="preserve">  login page</t>
   </si>
   <si>
@@ -88,6 +114,9 @@
     <t xml:space="preserve">  Testiranje UI</t>
   </si>
   <si>
+    <t xml:space="preserve">testiranje</t>
+  </si>
+  <si>
     <t xml:space="preserve">Komunikacija FE / BE i API: </t>
   </si>
   <si>
@@ -109,22 +138,25 @@
     <t xml:space="preserve">  app.py</t>
   </si>
   <si>
-    <t xml:space="preserve">app.py</t>
-  </si>
-  <si>
     <t xml:space="preserve">  ruter @app.route('/ruta1')</t>
   </si>
   <si>
-    <t xml:space="preserve">rang lista</t>
-  </si>
-  <si>
     <t xml:space="preserve">  kontroler def ruta1():</t>
   </si>
   <si>
     <t xml:space="preserve">def rang_lista()</t>
   </si>
   <si>
-    <t xml:space="preserve">  biznis logika / logovanje</t>
+    <t xml:space="preserve">logovanje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def login()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">čitanje tabela Users, Pitanja, Odgovori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vidi Pony i model.py</t>
   </si>
   <si>
     <t xml:space="preserve">  Deployment na Heroku</t>
@@ -133,7 +165,7 @@
     <t xml:space="preserve">  git repo za projekat</t>
   </si>
   <si>
-    <t xml:space="preserve">repo</t>
+    <t xml:space="preserve">admin za git/github</t>
   </si>
   <si>
     <t xml:space="preserve">  Deployment na Pythonanywhere.com</t>
@@ -142,9 +174,6 @@
     <t xml:space="preserve">Dokumentovanje koda</t>
   </si>
   <si>
-    <t xml:space="preserve">docs/BIM_TASKS.xlsx</t>
-  </si>
-  <si>
     <t xml:space="preserve">docs/resursi.txt</t>
   </si>
   <si>
@@ -163,13 +192,25 @@
     <t xml:space="preserve">model.py:Users.py</t>
   </si>
   <si>
-    <t xml:space="preserve">  Konekcija, conf, sqlite3</t>
+    <t xml:space="preserve">  Konekcija i konfiguracija na sqlite3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vidi Pony linkove</t>
   </si>
   <si>
     <t xml:space="preserve">  ORM Pony</t>
   </si>
   <si>
+    <t xml:space="preserve">modul za unos pitanja</t>
+  </si>
+  <si>
     <t xml:space="preserve">  Unos podataka u bazu (rucni ili automatski)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unos pitanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">izbor i provera pitanja</t>
   </si>
   <si>
     <t xml:space="preserve">  Testiranje </t>
@@ -182,7 +223,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -275,6 +316,13 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <color rgb="FFF58220"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -297,7 +345,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF666666"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -313,7 +361,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -401,7 +449,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -462,7 +510,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -474,12 +526,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -491,18 +539,38 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -515,6 +583,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -534,7 +606,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -551,7 +623,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FFA3238E"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -579,7 +651,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFF58220"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666666"/>
+      <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF00A65D"/>
@@ -599,10 +671,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -611,13 +683,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="8.19"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="12" style="0" width="8.19"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -655,6 +728,7 @@
       <c r="N1" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="O1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
@@ -679,7 +753,9 @@
       <c r="D3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="11"/>
+      <c r="E3" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -692,7 +768,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
@@ -708,7 +784,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
@@ -724,10 +800,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -742,10 +818,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="11"/>
@@ -760,7 +836,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
@@ -776,7 +852,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -786,15 +862,21 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
+      <c r="J9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
-        <v>22</v>
+      <c r="A10" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -810,12 +892,12 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D11" s="11"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16" t="s">
-        <v>24</v>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -828,11 +910,11 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="16"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -844,13 +926,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="16"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
@@ -861,8 +943,8 @@
       <c r="N13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17" t="s">
-        <v>27</v>
+      <c r="A14" s="18" t="s">
+        <v>29</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
@@ -877,16 +959,13 @@
       <c r="N14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18" t="s">
-        <v>28</v>
+      <c r="A15" s="19" t="s">
+        <v>30</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="19" t="s">
-        <v>29</v>
-      </c>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
@@ -896,13 +975,11 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
-      <c r="F16" s="21" t="s">
-        <v>31</v>
-      </c>
+      <c r="F16" s="21"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
@@ -931,12 +1008,14 @@
       <c r="N17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="22" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="F18" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="G18" s="21"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
@@ -947,13 +1026,15 @@
       <c r="N18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>35</v>
+      <c r="A19" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="23" t="s">
+        <v>37</v>
+      </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -963,16 +1044,14 @@
       <c r="N19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22" t="s">
-        <v>36</v>
+      <c r="A20" s="0" t="s">
+        <v>38</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="21"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="19" t="s">
-        <v>37</v>
-      </c>
+      <c r="G20" s="24"/>
+      <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
@@ -981,14 +1060,18 @@
       <c r="N20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22" t="s">
-        <v>38</v>
+      <c r="A21" s="25" t="s">
+        <v>39</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="21"/>
+      <c r="F21" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="24"/>
+      <c r="H21" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
@@ -997,91 +1080,92 @@
       <c r="N21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
+      <c r="A22" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
       <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="J22" s="25" t="s">
-        <v>41</v>
-      </c>
+      <c r="H22" s="21"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
       <c r="M22" s="11"/>
       <c r="N22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="30" t="s">
+        <v>43</v>
+      </c>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
     </row>
-    <row r="24" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="29" t="s">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="29" t="s">
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+    </row>
+    <row r="25" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="I24" s="29" t="s">
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="H25" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
+      <c r="I25" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
+      <c r="G26" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
       <c r="J26" s="11"/>
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
@@ -1090,37 +1174,63 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
+      <c r="A28" s="0" t="s">
+        <v>53</v>
+      </c>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
+      <c r="I28" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="J28" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="M28" s="35"/>
+      <c r="N28" s="35"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29" s="15"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1130,5 +1240,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sabiranje poena i upisivanje u rang listu
</commit_message>
<xml_diff>
--- a/docs/BIM_PROJEKAT_TASK_LIST.xlsx
+++ b/docs/BIM_PROJEKAT_TASK_LIST.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t xml:space="preserve">Petar</t>
   </si>
@@ -84,10 +84,10 @@
     <t xml:space="preserve">  main page</t>
   </si>
   <si>
-    <t xml:space="preserve">templates/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rang lista</t>
+    <t xml:space="preserve">templates/game.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sortirati rang listu</t>
   </si>
   <si>
     <t xml:space="preserve">  login page</t>
@@ -111,6 +111,9 @@
     <t xml:space="preserve">  JS iscrtavanje na ekranu (DOM)</t>
   </si>
   <si>
+    <t xml:space="preserve">jedno po jedno pitanje</t>
+  </si>
+  <si>
     <t xml:space="preserve">  Testiranje UI</t>
   </si>
   <si>
@@ -126,10 +129,10 @@
     <t xml:space="preserve">index.html/app.py</t>
   </si>
   <si>
-    <t xml:space="preserve">  JS ws:// send, receive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Python ws:// send, receive (opciono)</t>
+    <t xml:space="preserve">  JS na front endu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slanje odgovora na server</t>
   </si>
   <si>
     <t xml:space="preserve">Flask / backend</t>
@@ -162,6 +165,9 @@
     <t xml:space="preserve">  Deployment na Heroku</t>
   </si>
   <si>
+    <t xml:space="preserve">uraditi Deployment</t>
+  </si>
+  <si>
     <t xml:space="preserve">  git repo za projekat</t>
   </si>
   <si>
@@ -204,16 +210,10 @@
     <t xml:space="preserve">Users test podaci</t>
   </si>
   <si>
-    <t xml:space="preserve">Questions.txt Answers.txt</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Unos podataka u bazu (rucni ili automatski)</t>
   </si>
   <si>
     <t xml:space="preserve">unos pitanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">izbor i provera pitanja</t>
   </si>
   <si>
     <t xml:space="preserve">  Testiranje </t>
@@ -226,7 +226,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -317,6 +317,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -341,14 +348,15 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <color rgb="FFA09600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -452,7 +460,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -501,14 +509,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -517,11 +529,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -533,11 +545,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -549,15 +565,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -565,11 +589,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -577,14 +601,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -597,6 +621,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -605,7 +633,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -689,7 +717,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -700,7 +728,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.44"/>
@@ -785,8 +813,8 @@
       <c r="A4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -801,8 +829,8 @@
       <c r="A5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -817,7 +845,7 @@
       <c r="A6" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="11"/>
@@ -838,7 +866,7 @@
       <c r="D7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -854,7 +882,9 @@
         <v>21</v>
       </c>
       <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
+      <c r="E8" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -866,32 +896,32 @@
       <c r="N8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
+      <c r="A9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
+      <c r="J9" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="s">
-        <v>24</v>
+      <c r="A10" s="18" t="s">
+        <v>25</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -907,12 +937,12 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" s="11"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19" t="s">
-        <v>26</v>
+      <c r="E11" s="19"/>
+      <c r="F11" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -925,11 +955,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="18"/>
+      <c r="F12" s="21" t="s">
+        <v>29</v>
+      </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -940,14 +972,12 @@
       <c r="N12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="18"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
@@ -958,8 +988,8 @@
       <c r="N13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="s">
-        <v>29</v>
+      <c r="A14" s="22" t="s">
+        <v>30</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
@@ -974,8 +1004,8 @@
       <c r="N14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21" t="s">
-        <v>30</v>
+      <c r="A15" s="23" t="s">
+        <v>31</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
@@ -989,12 +1019,12 @@
       <c r="N15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22" t="s">
-        <v>31</v>
+      <c r="A16" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
-      <c r="F16" s="23"/>
+      <c r="F16" s="25"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
@@ -1005,14 +1035,14 @@
       <c r="N16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="22" t="s">
-        <v>32</v>
+      <c r="A17" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="24" t="s">
-        <v>33</v>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
@@ -1023,15 +1053,15 @@
       <c r="N17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="25" t="s">
-        <v>34</v>
+      <c r="A18" s="27" t="s">
+        <v>35</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="23"/>
+      <c r="F18" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="25"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
@@ -1041,14 +1071,14 @@
       <c r="N18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="25" t="s">
-        <v>36</v>
+      <c r="A19" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="24" t="s">
-        <v>37</v>
+      <c r="G19" s="29" t="s">
+        <v>38</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
@@ -1060,13 +1090,15 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="11"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
@@ -1075,17 +1107,17 @@
       <c r="N20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="27" t="s">
-        <v>39</v>
+      <c r="A21" s="31" t="s">
+        <v>41</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" s="26"/>
-      <c r="H21" s="28" t="s">
-        <v>40</v>
+      <c r="F21" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="30"/>
+      <c r="H21" s="32" t="s">
+        <v>42</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
@@ -1095,14 +1127,14 @@
       <c r="N21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="27" t="s">
-        <v>41</v>
+      <c r="A22" s="31" t="s">
+        <v>43</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="23"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="25"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
@@ -1111,19 +1143,19 @@
       <c r="N22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="32" t="s">
-        <v>43</v>
+      <c r="A23" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="36" t="s">
+        <v>45</v>
       </c>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
@@ -1131,13 +1163,13 @@
       <c r="N23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="33" t="s">
-        <v>44</v>
+      <c r="A24" s="37" t="s">
+        <v>46</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
-      <c r="G24" s="26"/>
+      <c r="G24" s="30"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
@@ -1146,41 +1178,41 @@
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
     </row>
-    <row r="25" s="34" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="H25" s="36" t="s">
+    <row r="25" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="I25" s="36" t="s">
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
+      <c r="H25" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="I25" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="39"/>
       <c r="O25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
-      <c r="G26" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
+      <c r="G26" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
       <c r="J26" s="11"/>
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
@@ -1189,19 +1221,17 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="I27" s="36"/>
-      <c r="J27" s="38" t="s">
-        <v>53</v>
-      </c>
+      <c r="G27" s="41"/>
+      <c r="H27" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" s="41"/>
+      <c r="J27" s="43"/>
       <c r="K27" s="11"/>
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
@@ -1209,45 +1239,47 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="J28" s="36" t="s">
+      <c r="F28" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="M28" s="36"/>
-      <c r="N28" s="36"/>
+      <c r="G28" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="J28" s="41"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="L29" s="16"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29" s="17"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>